<commit_message>
added lifeformwright to list
</commit_message>
<xml_diff>
--- a/splists_out/Wright_not_CurrentPanamaWoody_2026-02-20.xlsx
+++ b/splists_out/Wright_not_CurrentPanamaWoody_2026-02-20.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AL15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -543,6 +543,11 @@
           <t>is_alternate_name</t>
         </is>
       </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>lifeform_wright</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -706,6 +711,11 @@
       <c r="AK2" t="b">
         <v>0</v>
       </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>LIANA, CLIMBER</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -854,6 +864,11 @@
       <c r="AK3" t="b">
         <v>0</v>
       </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>UNDERSTORY, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1012,6 +1027,11 @@
       <c r="AK4" t="b">
         <v>0</v>
       </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>SHRUB, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1165,6 +1185,11 @@
       <c r="AK5" t="b">
         <v>0</v>
       </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>SHRUB, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1318,6 +1343,11 @@
       <c r="AK6" t="b">
         <v>0</v>
       </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>SHRUB, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1466,6 +1496,11 @@
       <c r="AK7" t="b">
         <v>0</v>
       </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>SHRUB, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1614,6 +1649,11 @@
       <c r="AK8" t="b">
         <v>0</v>
       </c>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t>SHRUB, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1772,6 +1812,11 @@
       <c r="AK9" t="b">
         <v>0</v>
       </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t>SHRUB, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1940,6 +1985,11 @@
       <c r="AK10" t="b">
         <v>0</v>
       </c>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t>SHRUB, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2093,6 +2143,11 @@
       <c r="AK11" t="b">
         <v>1</v>
       </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t>SHRUB, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2261,6 +2316,11 @@
       <c r="AK12" t="b">
         <v>0</v>
       </c>
+      <c r="AL12" t="inlineStr">
+        <is>
+          <t>UNDERSTORY, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2414,6 +2474,11 @@
       <c r="AK13" t="b">
         <v>1</v>
       </c>
+      <c r="AL13" t="inlineStr">
+        <is>
+          <t>LIANA, CLIMBER</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2547,6 +2612,11 @@
       <c r="AK14" t="b">
         <v>0</v>
       </c>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>TREE, FREE</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2704,6 +2774,11 @@
       </c>
       <c r="AK15" t="b">
         <v>0</v>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>SHRUB, FREE</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated column for synonym source in wright list for revision
</commit_message>
<xml_diff>
--- a/splists_out/Wright_not_CurrentPanamaWoody_2026-02-20.xlsx
+++ b/splists_out/Wright_not_CurrentPanamaWoody_2026-02-20.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL15"/>
+  <dimension ref="A1:AO15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -548,6 +548,21 @@
           <t>lifeform_wright</t>
         </is>
       </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>synonym_match_name</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>forestgeo_synonym_source</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>OriginalOrder</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2148,6 +2163,19 @@
           <t>SHRUB, FREE</t>
         </is>
       </c>
+      <c r="AM11" t="inlineStr">
+        <is>
+          <t>Ixora coccinea</t>
+        </is>
+      </c>
+      <c r="AN11" t="inlineStr">
+        <is>
+          <t>Ixora chinensis</t>
+        </is>
+      </c>
+      <c r="AO11">
+        <v>1364</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2478,6 +2506,19 @@
         <is>
           <t>LIANA, CLIMBER</t>
         </is>
+      </c>
+      <c r="AM13" t="inlineStr">
+        <is>
+          <t>Salacia multiflora</t>
+        </is>
+      </c>
+      <c r="AN13" t="inlineStr">
+        <is>
+          <t>Salacia polyantha</t>
+        </is>
+      </c>
+      <c r="AO13">
+        <v>2568</v>
       </c>
     </row>
     <row r="14">

</xml_diff>